<commit_message>
updated by Raafat Abdelkader
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/UsersData.xlsx
+++ b/src/test/resources/testData/UsersData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\E2E_Demo_Project\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB54503A-0572-4CE7-BF22-D47AD19C916D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560DCB48-0AD0-4746-84C8-C5F7B16F3684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>